<commit_message>
update Signed-off-by: LeeWJ <960457215@qq.com>
</commit_message>
<xml_diff>
--- a/关键字参数说明文档.xlsx
+++ b/关键字参数说明文档.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="170">
   <si>
     <t>名称</t>
   </si>
@@ -536,16 +536,22 @@
   <si>
     <t>纵坐标</t>
   </si>
+  <si>
+    <t>退出appium</t>
+  </si>
+  <si>
+    <t>注：当使用xpath locator时，如遇到多个相同匹配，使用以下方式进行匹配：%{数组下标}xpath表达式，例子：%{4}//*[@resource-id="cn.owhatlab:id/tv_buy_name"]，表明匹配第5个xpath</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -570,7 +576,108 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -584,7 +691,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -599,7 +706,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -611,107 +718,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -734,187 +740,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -943,6 +949,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -954,6 +999,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -981,65 +1046,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1048,149 +1054,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1220,6 +1226,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1584,305 +1593,305 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" ht="96" customHeight="1" spans="1:9">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" ht="57.6" spans="1:9">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="13"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" ht="28.8" spans="1:9">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" ht="28.8" spans="1:9">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" ht="43.2" spans="1:9">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" ht="72" spans="1:9">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" ht="57.6" spans="1:9">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" ht="43.2" spans="1:9">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" ht="43.2" spans="1:9">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" ht="115.2" spans="1:9">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" ht="115.2" spans="1:9">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="13"/>
+      <c r="I13" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1912,433 +1921,433 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:9">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" ht="43.2" spans="1:9">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" ht="96" customHeight="1" spans="1:9">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" ht="28.8" spans="1:9">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" ht="28.8" spans="1:9">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" ht="28.8" spans="1:9">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" ht="28.8" spans="1:9">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" ht="28.8" spans="1:9">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" ht="28.8" spans="1:9">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" ht="57.6" spans="1:9">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" ht="28.8" spans="1:9">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" ht="28.8" spans="1:9">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
     </row>
     <row r="16" ht="28.8" spans="1:9">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
     </row>
     <row r="18" ht="28.8" spans="1:9">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
     </row>
     <row r="19" ht="28.8" spans="1:9">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
     </row>
     <row r="20" ht="28.8" spans="1:9">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
     </row>
     <row r="21" ht="28.8" spans="1:9">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2349,10 +2358,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2646,7 +2655,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="6" t="s">
-        <v>103</v>
+        <v>168</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>104</v>
@@ -2659,7 +2668,23 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
+    <row r="15" ht="34" customHeight="1" spans="1:9">
+      <c r="A15" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:I15"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>